<commit_message>
added report tab in main
</commit_message>
<xml_diff>
--- a/imap_client_app/bin/Debug/attachments/CAL68X71M+mzYRUOkunKbDBX6938O_rT0=9suOXQoguKXs4czBg@mail.gmail.com/test_data.xlsx
+++ b/imap_client_app/bin/Debug/attachments/CAL68X71M+mzYRUOkunKbDBX6938O_rT0=9suOXQoguKXs4czBg@mail.gmail.com/test_data.xlsx
@@ -363,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D17"/>
+  <dimension ref="B4:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D17"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -374,179 +374,179 @@
     <col min="4" max="4" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
-      <c r="B2" t="s">
+    <row r="4" spans="2:4">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D4" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4">
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1">
-        <v>41924</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4">
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1">
-        <v>41925</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="1">
-        <v>41926</v>
+        <v>41924</v>
       </c>
     </row>
     <row r="6" spans="2:4">
       <c r="B6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="1">
-        <v>41927</v>
+        <v>41925</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="1">
-        <v>41928</v>
+        <v>41926</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="1">
-        <v>41929</v>
+        <v>41927</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="1">
-        <v>41930</v>
+        <v>41928</v>
       </c>
     </row>
     <row r="10" spans="2:4">
       <c r="B10">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="1">
-        <v>41931</v>
+        <v>41929</v>
       </c>
     </row>
     <row r="11" spans="2:4">
       <c r="B11">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="1">
-        <v>41932</v>
+        <v>41930</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="B12">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="1">
-        <v>41933</v>
+        <v>41931</v>
       </c>
     </row>
     <row r="13" spans="2:4">
       <c r="B13">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="1">
-        <v>41934</v>
+        <v>41932</v>
       </c>
     </row>
     <row r="14" spans="2:4">
       <c r="B14">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="1">
-        <v>41935</v>
+        <v>41933</v>
       </c>
     </row>
     <row r="15" spans="2:4">
       <c r="B15">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="1">
-        <v>41936</v>
+        <v>41934</v>
       </c>
     </row>
     <row r="16" spans="2:4">
       <c r="B16">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="1">
-        <v>41937</v>
+        <v>41935</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1">
+        <v>41936</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="1">
+        <v>41937</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19">
         <v>15</v>
       </c>
-      <c r="C17" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="1">
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1">
         <v>41938</v>
       </c>
     </row>

</xml_diff>